<commit_message>
extracted duplicates from kth-data
</commit_message>
<xml_diff>
--- a/data/kth/original_data/2017_OpenAPC_Sweden_Agresso_table.xlsx
+++ b/data/kth/original_data/2017_OpenAPC_Sweden_Agresso_table.xlsx
@@ -12,14 +12,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="300"/>
   </bookViews>
   <sheets>
-    <sheet name="2017_OpenAPC_Sweden_Agresso" sheetId="1" r:id="rId1"/>
+    <sheet name="2017_utan_dubbletter" sheetId="3" r:id="rId1"/>
+    <sheet name="2017_OpenAPC_Sweden_Agresso" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="147">
   <si>
     <t>institution</t>
   </si>
@@ -997,7 +998,43 @@
     <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Varningstext" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1020,7 +1057,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F139" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:F117" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F117"/>
+  <sortState ref="A2:F162">
+    <sortCondition sortBy="cellColor" ref="D2:D162" dxfId="2"/>
+    <sortCondition ref="C2:C162"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="institution"/>
+    <tableColumn id="2" name="period"/>
+    <tableColumn id="3" name="euro"/>
+    <tableColumn id="4" name="doi"/>
+    <tableColumn id="5" name="is_hybrid"/>
+    <tableColumn id="6" name="publisher"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F139" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:F139"/>
   <sortState ref="A2:E139">
     <sortCondition ref="D2:D139"/>
@@ -1300,7 +1356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1341,6 +1397,2028 @@
         <v>2017</v>
       </c>
       <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2017</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2017</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2017</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2017</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2017</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2017</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>2017</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>2017</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2017</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>2017</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2017</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2017</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2017</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>2017</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2017</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>2017</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2017</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2017</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>2017</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>2017</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>2017</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2017</v>
+      </c>
+      <c r="C24">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>2017</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>2017</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>2017</v>
+      </c>
+      <c r="C27">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>2017</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>2017</v>
+      </c>
+      <c r="C29">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>2017</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>2017</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>2017</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>2017</v>
+      </c>
+      <c r="C33">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>2017</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>2017</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>2017</v>
+      </c>
+      <c r="C36">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>2017</v>
+      </c>
+      <c r="C37">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>2017</v>
+      </c>
+      <c r="C38">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>2017</v>
+      </c>
+      <c r="C39">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>2017</v>
+      </c>
+      <c r="C40">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>2017</v>
+      </c>
+      <c r="C41">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>2017</v>
+      </c>
+      <c r="C42">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>2017</v>
+      </c>
+      <c r="C43">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>2017</v>
+      </c>
+      <c r="C44">
+        <v>260</v>
+      </c>
+      <c r="D44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>2017</v>
+      </c>
+      <c r="C45">
+        <v>300</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>2017</v>
+      </c>
+      <c r="C46">
+        <v>360</v>
+      </c>
+      <c r="D46" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>2017</v>
+      </c>
+      <c r="C47">
+        <v>420</v>
+      </c>
+      <c r="D47" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>2017</v>
+      </c>
+      <c r="C48">
+        <v>449</v>
+      </c>
+      <c r="D48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>2017</v>
+      </c>
+      <c r="C49">
+        <v>449</v>
+      </c>
+      <c r="D49" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>2017</v>
+      </c>
+      <c r="C50">
+        <v>449</v>
+      </c>
+      <c r="D50" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>2017</v>
+      </c>
+      <c r="C51">
+        <v>449</v>
+      </c>
+      <c r="D51" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>2017</v>
+      </c>
+      <c r="C52">
+        <v>466</v>
+      </c>
+      <c r="D52" t="s">
+        <v>112</v>
+      </c>
+      <c r="E52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>2017</v>
+      </c>
+      <c r="C53">
+        <v>520</v>
+      </c>
+      <c r="D53" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>2017</v>
+      </c>
+      <c r="C54">
+        <v>525</v>
+      </c>
+      <c r="D54" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>2017</v>
+      </c>
+      <c r="C55">
+        <v>639</v>
+      </c>
+      <c r="D55" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>2017</v>
+      </c>
+      <c r="C56">
+        <v>647</v>
+      </c>
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>2017</v>
+      </c>
+      <c r="C57">
+        <v>660</v>
+      </c>
+      <c r="D57" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>2017</v>
+      </c>
+      <c r="C58">
+        <v>818</v>
+      </c>
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>2017</v>
+      </c>
+      <c r="C59">
+        <v>987</v>
+      </c>
+      <c r="D59" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>2017</v>
+      </c>
+      <c r="C60">
+        <v>1050</v>
+      </c>
+      <c r="D60" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>2017</v>
+      </c>
+      <c r="C61">
+        <v>1050</v>
+      </c>
+      <c r="D61" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>2017</v>
+      </c>
+      <c r="C62">
+        <v>1050</v>
+      </c>
+      <c r="D62" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>2017</v>
+      </c>
+      <c r="C63">
+        <v>1050</v>
+      </c>
+      <c r="D63" t="s">
+        <v>39</v>
+      </c>
+      <c r="E63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>2017</v>
+      </c>
+      <c r="C64">
+        <v>1075</v>
+      </c>
+      <c r="D64" t="s">
+        <v>31</v>
+      </c>
+      <c r="E64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>2017</v>
+      </c>
+      <c r="C65">
+        <v>1165</v>
+      </c>
+      <c r="D65" t="s">
+        <v>125</v>
+      </c>
+      <c r="E65" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>2017</v>
+      </c>
+      <c r="C66">
+        <v>1165</v>
+      </c>
+      <c r="D66" t="s">
+        <v>66</v>
+      </c>
+      <c r="E66" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>2017</v>
+      </c>
+      <c r="C67">
+        <v>1201</v>
+      </c>
+      <c r="D67" t="s">
+        <v>138</v>
+      </c>
+      <c r="E67" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>2017</v>
+      </c>
+      <c r="C68">
+        <v>1203</v>
+      </c>
+      <c r="D68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>2017</v>
+      </c>
+      <c r="C69">
+        <v>1220</v>
+      </c>
+      <c r="D69" t="s">
+        <v>139</v>
+      </c>
+      <c r="E69" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>2017</v>
+      </c>
+      <c r="C70">
+        <v>1274</v>
+      </c>
+      <c r="D70" t="s">
+        <v>55</v>
+      </c>
+      <c r="E70" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>2017</v>
+      </c>
+      <c r="C71">
+        <v>1278</v>
+      </c>
+      <c r="D71" t="s">
+        <v>47</v>
+      </c>
+      <c r="E71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>2017</v>
+      </c>
+      <c r="C72">
+        <v>1305</v>
+      </c>
+      <c r="D72" t="s">
+        <v>122</v>
+      </c>
+      <c r="E72" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>2017</v>
+      </c>
+      <c r="C73">
+        <v>1305</v>
+      </c>
+      <c r="D73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74">
+        <v>2017</v>
+      </c>
+      <c r="C74">
+        <v>1305</v>
+      </c>
+      <c r="D74" t="s">
+        <v>126</v>
+      </c>
+      <c r="E74" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>2017</v>
+      </c>
+      <c r="C75">
+        <v>1305</v>
+      </c>
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>2017</v>
+      </c>
+      <c r="C76">
+        <v>1305</v>
+      </c>
+      <c r="D76" t="s">
+        <v>114</v>
+      </c>
+      <c r="E76" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>2017</v>
+      </c>
+      <c r="C77">
+        <v>1305</v>
+      </c>
+      <c r="D77" t="s">
+        <v>123</v>
+      </c>
+      <c r="E77" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>2017</v>
+      </c>
+      <c r="C78">
+        <v>1305</v>
+      </c>
+      <c r="D78" t="s">
+        <v>65</v>
+      </c>
+      <c r="E78" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>2017</v>
+      </c>
+      <c r="C79">
+        <v>1305</v>
+      </c>
+      <c r="D79" t="s">
+        <v>124</v>
+      </c>
+      <c r="E79" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>2017</v>
+      </c>
+      <c r="C80">
+        <v>1328</v>
+      </c>
+      <c r="D80" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>2017</v>
+      </c>
+      <c r="C81">
+        <v>1336</v>
+      </c>
+      <c r="D81" t="s">
+        <v>137</v>
+      </c>
+      <c r="E81" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>2017</v>
+      </c>
+      <c r="C82">
+        <v>1372</v>
+      </c>
+      <c r="D82" t="s">
+        <v>135</v>
+      </c>
+      <c r="E82" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>2017</v>
+      </c>
+      <c r="C83">
+        <v>1403</v>
+      </c>
+      <c r="D83" t="s">
+        <v>142</v>
+      </c>
+      <c r="E83" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84">
+        <v>2017</v>
+      </c>
+      <c r="C84">
+        <v>1497</v>
+      </c>
+      <c r="D84" t="s">
+        <v>140</v>
+      </c>
+      <c r="E84" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>2017</v>
+      </c>
+      <c r="C85">
+        <v>1535</v>
+      </c>
+      <c r="D85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>2017</v>
+      </c>
+      <c r="C86">
+        <v>1603</v>
+      </c>
+      <c r="D86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E86" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>2017</v>
+      </c>
+      <c r="C87">
+        <v>1611</v>
+      </c>
+      <c r="D87" t="s">
+        <v>43</v>
+      </c>
+      <c r="E87" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88">
+        <v>2017</v>
+      </c>
+      <c r="C88">
+        <v>1615</v>
+      </c>
+      <c r="D88" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>2017</v>
+      </c>
+      <c r="C89">
+        <v>1713</v>
+      </c>
+      <c r="D89" t="s">
+        <v>51</v>
+      </c>
+      <c r="E89" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>2017</v>
+      </c>
+      <c r="C90">
+        <v>1755</v>
+      </c>
+      <c r="D90" t="s">
+        <v>44</v>
+      </c>
+      <c r="E90" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>2017</v>
+      </c>
+      <c r="C91">
+        <v>1837</v>
+      </c>
+      <c r="D91" t="s">
+        <v>53</v>
+      </c>
+      <c r="E91" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>2017</v>
+      </c>
+      <c r="C92">
+        <v>1837</v>
+      </c>
+      <c r="D92" t="s">
+        <v>54</v>
+      </c>
+      <c r="E92" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>2017</v>
+      </c>
+      <c r="C93">
+        <v>2040</v>
+      </c>
+      <c r="D93" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>2017</v>
+      </c>
+      <c r="C94">
+        <v>2192</v>
+      </c>
+      <c r="D94" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>2017</v>
+      </c>
+      <c r="C95">
+        <v>2227</v>
+      </c>
+      <c r="D95" t="s">
+        <v>45</v>
+      </c>
+      <c r="E95" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>2017</v>
+      </c>
+      <c r="C96">
+        <v>2243</v>
+      </c>
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>2017</v>
+      </c>
+      <c r="C97">
+        <v>2243</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98">
+        <v>2017</v>
+      </c>
+      <c r="C98">
+        <v>2243</v>
+      </c>
+      <c r="D98" t="s">
+        <v>23</v>
+      </c>
+      <c r="E98" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99">
+        <v>2017</v>
+      </c>
+      <c r="C99">
+        <v>2243</v>
+      </c>
+      <c r="D99" t="s">
+        <v>14</v>
+      </c>
+      <c r="E99" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>2017</v>
+      </c>
+      <c r="C100">
+        <v>2243</v>
+      </c>
+      <c r="D100" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101">
+        <v>2017</v>
+      </c>
+      <c r="C101">
+        <v>2500</v>
+      </c>
+      <c r="D101" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102">
+        <v>2017</v>
+      </c>
+      <c r="C102">
+        <v>2500</v>
+      </c>
+      <c r="D102" t="s">
+        <v>17</v>
+      </c>
+      <c r="E102" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103">
+        <v>2017</v>
+      </c>
+      <c r="C103">
+        <v>2691</v>
+      </c>
+      <c r="D103" t="s">
+        <v>61</v>
+      </c>
+      <c r="E103" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104">
+        <v>2017</v>
+      </c>
+      <c r="C104">
+        <v>2691</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105">
+        <v>2017</v>
+      </c>
+      <c r="C105">
+        <v>2750</v>
+      </c>
+      <c r="D105" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106">
+        <v>2017</v>
+      </c>
+      <c r="C106">
+        <v>2781</v>
+      </c>
+      <c r="D106" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107">
+        <v>2017</v>
+      </c>
+      <c r="C107">
+        <v>2796</v>
+      </c>
+      <c r="D107" t="s">
+        <v>25</v>
+      </c>
+      <c r="E107" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108">
+        <v>2017</v>
+      </c>
+      <c r="C108">
+        <v>2800</v>
+      </c>
+      <c r="D108" t="s">
+        <v>67</v>
+      </c>
+      <c r="E108" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109">
+        <v>2017</v>
+      </c>
+      <c r="C109">
+        <v>2871</v>
+      </c>
+      <c r="D109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E109" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110">
+        <v>2017</v>
+      </c>
+      <c r="C110">
+        <v>2871</v>
+      </c>
+      <c r="D110" t="s">
+        <v>20</v>
+      </c>
+      <c r="E110" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111">
+        <v>2017</v>
+      </c>
+      <c r="C111">
+        <v>2871</v>
+      </c>
+      <c r="D111" t="s">
+        <v>26</v>
+      </c>
+      <c r="E111" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112">
+        <v>2017</v>
+      </c>
+      <c r="C112">
+        <v>2960</v>
+      </c>
+      <c r="D112" t="s">
+        <v>28</v>
+      </c>
+      <c r="E112" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113">
+        <v>2017</v>
+      </c>
+      <c r="C113">
+        <v>3382</v>
+      </c>
+      <c r="D113" t="s">
+        <v>40</v>
+      </c>
+      <c r="E113" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114">
+        <v>2017</v>
+      </c>
+      <c r="C114">
+        <v>3409</v>
+      </c>
+      <c r="D114" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115">
+        <v>2017</v>
+      </c>
+      <c r="C115">
+        <v>3409</v>
+      </c>
+      <c r="D115" t="s">
+        <v>22</v>
+      </c>
+      <c r="E115" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116">
+        <v>2017</v>
+      </c>
+      <c r="C116">
+        <v>3700</v>
+      </c>
+      <c r="D116" t="s">
+        <v>62</v>
+      </c>
+      <c r="E116" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117">
+        <v>2017</v>
+      </c>
+      <c r="C117">
+        <v>3700</v>
+      </c>
+      <c r="D117" t="s">
+        <v>121</v>
+      </c>
+      <c r="E117" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D96:D117">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F140"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2017</v>
+      </c>
+      <c r="C2">
         <v>2500</v>
       </c>
       <c r="D2" t="s">

</xml_diff>